<commit_message>
3d foot in the making :)
</commit_message>
<xml_diff>
--- a/gui/Flash/footShape.xlsx
+++ b/gui/Flash/footShape.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="11895"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19020" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,6 +59,53 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>52922</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect l="58125" t="13675" r="22344" b="27457"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7877175" y="2338922"/>
+          <a:ext cx="2962275" cy="6528854"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -19523,7 +19570,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
         <a:srcRect l="60105" t="6240" r="9156"/>
         <a:stretch>
           <a:fillRect/>
@@ -36550,6 +36597,1304 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="550" name="Oval 549"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8410575" y="2809875"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="551" name="Oval 550"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9820275" y="3257550"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="552" name="Oval 551"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9096375" y="3048000"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="553" name="Oval 552"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9582150" y="4210050"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="554" name="Oval 553"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="5638800"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="555" name="Oval 554"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9096375" y="5657850"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="556" name="Oval 555"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9801225" y="5876925"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="557" name="Oval 556"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8629650" y="3971925"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="558" name="Oval 557"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8420100" y="4667250"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="559" name="Oval 558"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9324975" y="4933950"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="560" name="Oval 559"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9553575" y="6610350"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="561" name="Oval 560"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8620125" y="6600825"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="562" name="Oval 561"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8401050" y="8010525"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="563" name="Oval 562"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9334500" y="8020050"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="564" name="Oval 563"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9086850" y="7305675"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="565" name="Oval 564"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9810750" y="4695825"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="566" name="Rectangle 565"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8162925" y="3657600"/>
+          <a:ext cx="2314575" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="567" name="Rectangle 566"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7029450" y="5838825"/>
+          <a:ext cx="2314575" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="568" name="Rectangle 567"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="9105900" y="5715000"/>
+          <a:ext cx="2314575" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-CA" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="570" name="Straight Connector 569"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8658225" y="6362700"/>
+          <a:ext cx="2590800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="571" name="Straight Connector 570"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8658225" y="3962400"/>
+          <a:ext cx="2590800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="572" name="Straight Connector 571"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7724775" y="7534275"/>
+          <a:ext cx="2590800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="573" name="Straight Connector 572"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7686675" y="5153025"/>
+          <a:ext cx="2590800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -36842,8 +38187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="M16" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>